<commit_message>
Fixed more winner odds BUGs
</commit_message>
<xml_diff>
--- a/data/cwc2023.group_stage.odi_list.xlsx
+++ b/data/cwc2023.group_stage.odi_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Not.Dropbox\CODING\js_react\cwc2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64334E21-6404-4B41-8280-B97877B5AF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D619E5-D47A-4CF9-9984-995DF18241AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="-15345" windowWidth="24540" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1125,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="M2" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,7 +1138,7 @@
     <col min="12" max="12" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1203,11 +1203,11 @@
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="1" t="str">
-        <f>""""&amp;A2&amp;""":  {[TEAM."&amp;E2&amp;".id]: "&amp;H2&amp;", [TEAM."&amp;F2&amp;".id]: "&amp;I2&amp;"},  //  "&amp;J2&amp;"-"&amp;K2</f>
-        <v>"ODI 01":  {[TEAM.ENG.id]: 1.8, [TEAM.NZL.id]: 2.2},  //  OC-45204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <f>""""&amp;A2&amp;""":  {[TEAM."&amp;E2&amp;".id]: "&amp;H2&amp;", [TEAM."&amp;F2&amp;".id]: "&amp;I2&amp;"},  // "&amp;J2&amp;"-"&amp;K2</f>
+        <v>"ODI 01":  {[TEAM.ENG.id]: 1.8, [TEAM.NZL.id]: 2.2},  // OC-45204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1240,11 +1240,11 @@
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="1" t="str">
-        <f t="shared" ref="M3:M11" si="0">""""&amp;A3&amp;""":  {[TEAM."&amp;E3&amp;".id]: "&amp;H3&amp;", [TEAM."&amp;F3&amp;".id]: "&amp;I3&amp;"},  //  "&amp;J3&amp;"-"&amp;K3</f>
-        <v>"ODI 02":  {[TEAM.PAK.id]: 1.04, [TEAM.NLD.id]: 11.05},  //  OC-45205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+        <f t="shared" ref="M3:M11" si="0">""""&amp;A3&amp;""":  {[TEAM."&amp;E3&amp;".id]: "&amp;H3&amp;", [TEAM."&amp;F3&amp;".id]: "&amp;I3&amp;"},  // "&amp;J3&amp;"-"&amp;K3</f>
+        <v>"ODI 02":  {[TEAM.PAK.id]: 1.04, [TEAM.NLD.id]: 11.05},  // OC-45205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1279,16 +1279,10 @@
       <c r="L4" s="7"/>
       <c r="M4" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 03":  {[TEAM.AFG.id]: 2.5, [TEAM.BGD.id]: 1.8},  //  OC-2023-10-07</v>
-      </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 03":  {[TEAM.AFG.id]: 2.5, [TEAM.BGD.id]: 1.8},  // OC-2023-10-07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1323,16 +1317,10 @@
       <c r="L5" s="7"/>
       <c r="M5" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 04":  {[TEAM.ZAF.id]: 1.44, [TEAM.LKA.id]: 3.1},  //  OC-2023-10-07</v>
-      </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 04":  {[TEAM.ZAF.id]: 1.44, [TEAM.LKA.id]: 3.1},  // OC-2023-10-07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1367,16 +1355,10 @@
       <c r="L6" s="7"/>
       <c r="M6" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 05":  {[TEAM.AUS.id]: 2.37, [TEAM.IND.id]: 1.67},  //  OC-2023-10-07</v>
-      </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 05":  {[TEAM.AUS.id]: 2.37, [TEAM.IND.id]: 1.67},  // OC-2023-10-07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1411,16 +1393,10 @@
       <c r="L7" s="7"/>
       <c r="M7" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 06":  {[TEAM.NZL.id]: 1.06, [TEAM.NLD.id]: 11},  //  OC-2023-10-07</v>
-      </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 06":  {[TEAM.NZL.id]: 1.06, [TEAM.NLD.id]: 11},  // OC-2023-10-07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1455,16 +1431,10 @@
       <c r="L8" s="7"/>
       <c r="M8" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 07":  {[TEAM.BGD.id]: 4.8, [TEAM.ENG.id]: 1.18},  //  OP-2023-10-07</v>
-      </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 07":  {[TEAM.BGD.id]: 4.8, [TEAM.ENG.id]: 1.18},  // OP-2023-10-07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1499,16 +1469,10 @@
       <c r="L9" s="7"/>
       <c r="M9" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 08":  {[TEAM.PAK.id]: 1.46, [TEAM.LKA.id]: 2.73},  //  OP-2023-10-07</v>
-      </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 08":  {[TEAM.PAK.id]: 1.46, [TEAM.LKA.id]: 2.73},  // OP-2023-10-07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1543,16 +1507,10 @@
       <c r="L10" s="7"/>
       <c r="M10" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 09":  {[TEAM.AFG.id]: 5.1, [TEAM.IND.id]: 1.17},  //  OP-2023-10-07</v>
-      </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 09":  {[TEAM.AFG.id]: 5.1, [TEAM.IND.id]: 1.17},  // OP-2023-10-07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1587,16 +1545,10 @@
       <c r="L11" s="7"/>
       <c r="M11" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>"ODI 10":  {[TEAM.AUS.id]: 1.63, [TEAM.ZAF.id]: 2.29},  //  OP-2023-10-07</v>
-      </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>"ODI 10":  {[TEAM.AUS.id]: 1.63, [TEAM.ZAF.id]: 2.29},  // OP-2023-10-07</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1616,7 +1568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +1588,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1656,7 +1608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1676,7 +1628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>38</v>
       </c>

</xml_diff>